<commit_message>
7008, 7009, 7010 preprocessing
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" uniqueCount="8">
   <si>
     <t>7002</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>7007</t>
+  </si>
+  <si>
+    <t>7008</t>
+  </si>
+  <si>
+    <t>7009</t>
+  </si>
+  <si>
+    <t>7010</t>
   </si>
 </sst>
 </file>
@@ -73,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B7"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -115,6 +124,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
preprocessed and epoched 7025 (and 7028 and 7029)
ICA for 7028 and 7030 were taking forever and im not sure why so they couldn't be preprocessed, 7028 and 7029 were processed but will not be incorporated into analyses due to lack of trials
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>7002</t>
   </si>
@@ -49,6 +49,24 @@
   </si>
   <si>
     <t>7024</t>
+  </si>
+  <si>
+    <t>7025</t>
+  </si>
+  <si>
+    <t>7025</t>
+  </si>
+  <si>
+    <t>7027</t>
+  </si>
+  <si>
+    <t>7028</t>
+  </si>
+  <si>
+    <t>7029</t>
+  </si>
+  <si>
+    <t>7030</t>
   </si>
 </sst>
 </file>
@@ -102,14 +120,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B24"/>
+  <dimension ref="A3:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.15625" customWidth="true"/>
-    <col min="2" max="2" width="2.15625" customWidth="true"/>
+    <col min="1" max="1" width="5.16796875" customWidth="true"/>
+    <col min="2" max="2" width="2.16796875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -192,6 +210,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="0">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resyncing with pitt computer
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="19">
   <si>
     <t>7002</t>
   </si>
@@ -67,12 +67,15 @@
   </si>
   <si>
     <t>7030</t>
+  </si>
+  <si>
+    <t>7033</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -120,14 +123,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B30"/>
+  <dimension ref="A3:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.16796875" customWidth="true"/>
-    <col min="2" max="2" width="2.16796875" customWidth="true"/>
+    <col min="1" max="1" width="5.140625" customWidth="true"/>
+    <col min="2" max="2" width="2.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="3">
@@ -247,7 +250,15 @@
         <v>17</v>
       </c>
       <c r="B30" s="0">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
discovering issue!! going to repreprocess!!!
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="22" uniqueCount="20">
   <si>
     <t>7002</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>7033</t>
+  </si>
+  <si>
+    <t>7038</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B33"/>
+  <dimension ref="A3:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -261,6 +264,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="0">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>